<commit_message>
Add functions to freeze cells and add filters in Excel spreadsheets
</commit_message>
<xml_diff>
--- a/04_Practical_Projects/files/openpyxl_files/hello_world.xlsx
+++ b/04_Practical_Projects/files/openpyxl_files/hello_world.xlsx
@@ -416,7 +416,10 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AE12" sqref="AE12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -511,7 +514,14 @@
   <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>

</xml_diff>